<commit_message>
Update standard_dict - V4_1.31.xlsx
</commit_message>
<xml_diff>
--- a/doc/KeyV4.1/standard_dict - V4_1.31.xlsx
+++ b/doc/KeyV4.1/standard_dict - V4_1.31.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Method1" sheetId="1" r:id="rId1"/>
@@ -6401,8 +6401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ836"/>
   <sheetViews>
-    <sheetView topLeftCell="A767" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I786" sqref="I786"/>
+    <sheetView topLeftCell="A674" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E684" sqref="E684"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30669,8 +30669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G925"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A533" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30:B560"/>
+    <sheetView topLeftCell="A521" workbookViewId="0">
+      <selection activeCell="D528" sqref="D528"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30715,7 +30715,7 @@
       </c>
       <c r="D2" s="1">
         <f>VLOOKUP(B2,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E2" s="3">
         <f t="shared" ref="E2:E65" si="0">ROUND(D2/C2*100000*F2/2.5,10)/IF(G2=TRUE(),2,1)</f>
@@ -30723,7 +30723,7 @@
       </c>
       <c r="F2" s="1">
         <f>VLOOKUP(B2,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G2" s="1" t="b">
         <f>FALSE()</f>
@@ -30743,7 +30743,7 @@
       </c>
       <c r="D3" s="1">
         <f>VLOOKUP(B3,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E3" s="3">
         <f t="shared" si="0"/>
@@ -30751,7 +30751,7 @@
       </c>
       <c r="F3" s="1">
         <f>VLOOKUP(B3,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G3" s="1" t="b">
         <f>FALSE()</f>
@@ -30771,7 +30771,7 @@
       </c>
       <c r="D4" s="1">
         <f>VLOOKUP(B4,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E4" s="3">
         <f t="shared" si="0"/>
@@ -30779,7 +30779,7 @@
       </c>
       <c r="F4" s="1">
         <f>VLOOKUP(B4,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G4" s="1" t="b">
         <f>FALSE()</f>
@@ -30799,7 +30799,7 @@
       </c>
       <c r="D5" s="1">
         <f>VLOOKUP(B5,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E5" s="3">
         <f t="shared" si="0"/>
@@ -30807,7 +30807,7 @@
       </c>
       <c r="F5" s="1">
         <f>VLOOKUP(B5,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G5" s="1" t="b">
         <f>FALSE()</f>
@@ -30827,7 +30827,7 @@
       </c>
       <c r="D6" s="1">
         <f>VLOOKUP(B6,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E6" s="3">
         <f t="shared" si="0"/>
@@ -30835,7 +30835,7 @@
       </c>
       <c r="F6" s="1">
         <f>VLOOKUP(B6,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G6" s="1" t="b">
         <f>FALSE()</f>
@@ -30855,7 +30855,7 @@
       </c>
       <c r="D7" s="1">
         <f>VLOOKUP(B7,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E7" s="3">
         <f t="shared" si="0"/>
@@ -30863,7 +30863,7 @@
       </c>
       <c r="F7" s="1">
         <f>VLOOKUP(B7,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G7" s="1" t="b">
         <f>FALSE()</f>
@@ -30883,7 +30883,7 @@
       </c>
       <c r="D8" s="1">
         <f>VLOOKUP(B8,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E8" s="3">
         <f t="shared" si="0"/>
@@ -30891,7 +30891,7 @@
       </c>
       <c r="F8" s="1">
         <f>VLOOKUP(B8,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G8" s="1" t="b">
         <f>FALSE()</f>
@@ -30911,7 +30911,7 @@
       </c>
       <c r="D9" s="1">
         <f>VLOOKUP(B9,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E9" s="3">
         <f t="shared" si="0"/>
@@ -30919,7 +30919,7 @@
       </c>
       <c r="F9" s="1">
         <f>VLOOKUP(B9,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G9" s="1" t="b">
         <f>FALSE()</f>
@@ -30939,7 +30939,7 @@
       </c>
       <c r="D10" s="1">
         <f>VLOOKUP(B10,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E10" s="3">
         <f t="shared" si="0"/>
@@ -30947,7 +30947,7 @@
       </c>
       <c r="F10" s="1">
         <f>VLOOKUP(B10,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G10" s="1" t="b">
         <f>FALSE()</f>
@@ -30967,7 +30967,7 @@
       </c>
       <c r="D11" s="1">
         <f>VLOOKUP(B11,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E11" s="3">
         <f t="shared" si="0"/>
@@ -30975,7 +30975,7 @@
       </c>
       <c r="F11" s="1">
         <f>VLOOKUP(B11,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G11" s="1" t="b">
         <f>FALSE()</f>
@@ -30995,7 +30995,7 @@
       </c>
       <c r="D12" s="1">
         <f>VLOOKUP(B12,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E12" s="3">
         <f t="shared" si="0"/>
@@ -31003,7 +31003,7 @@
       </c>
       <c r="F12" s="1">
         <f>VLOOKUP(B12,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G12" s="1" t="b">
         <f>FALSE()</f>
@@ -31023,7 +31023,7 @@
       </c>
       <c r="D13" s="1">
         <f>VLOOKUP(B13,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E13" s="3">
         <f t="shared" si="0"/>
@@ -31031,7 +31031,7 @@
       </c>
       <c r="F13" s="1">
         <f>VLOOKUP(B13,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G13" s="1" t="b">
         <f>FALSE()</f>
@@ -31051,7 +31051,7 @@
       </c>
       <c r="D14" s="1">
         <f>VLOOKUP(B14,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E14" s="3">
         <f t="shared" si="0"/>
@@ -31059,7 +31059,7 @@
       </c>
       <c r="F14" s="1">
         <f>VLOOKUP(B14,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G14" s="1" t="b">
         <f>FALSE()</f>
@@ -31079,7 +31079,7 @@
       </c>
       <c r="D15" s="1">
         <f>VLOOKUP(B15,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E15" s="3">
         <f t="shared" si="0"/>
@@ -31087,7 +31087,7 @@
       </c>
       <c r="F15" s="1">
         <f>VLOOKUP(B15,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G15" s="1" t="b">
         <f>FALSE()</f>
@@ -31107,7 +31107,7 @@
       </c>
       <c r="D16" s="1">
         <f>VLOOKUP(B16,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E16" s="3">
         <f t="shared" si="0"/>
@@ -31115,7 +31115,7 @@
       </c>
       <c r="F16" s="1">
         <f>VLOOKUP(B16,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G16" s="1" t="b">
         <f>FALSE()</f>
@@ -31135,7 +31135,7 @@
       </c>
       <c r="D17" s="1">
         <f>VLOOKUP(B17,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E17" s="3">
         <f t="shared" si="0"/>
@@ -31143,7 +31143,7 @@
       </c>
       <c r="F17" s="1">
         <f>VLOOKUP(B17,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G17" s="1" t="b">
         <f>FALSE()</f>
@@ -31163,7 +31163,7 @@
       </c>
       <c r="D18" s="1">
         <f>VLOOKUP(B18,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E18" s="3">
         <f t="shared" si="0"/>
@@ -31171,7 +31171,7 @@
       </c>
       <c r="F18" s="1">
         <f>VLOOKUP(B18,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G18" s="1" t="b">
         <f>FALSE()</f>
@@ -31191,7 +31191,7 @@
       </c>
       <c r="D19" s="1">
         <f>VLOOKUP(B19,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E19" s="3">
         <f t="shared" si="0"/>
@@ -31199,7 +31199,7 @@
       </c>
       <c r="F19" s="1">
         <f>VLOOKUP(B19,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G19" s="1" t="b">
         <f>FALSE()</f>
@@ -31219,7 +31219,7 @@
       </c>
       <c r="D20" s="1">
         <f>VLOOKUP(B20,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E20" s="3">
         <f t="shared" si="0"/>
@@ -31227,7 +31227,7 @@
       </c>
       <c r="F20" s="1">
         <f>VLOOKUP(B20,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G20" s="1" t="b">
         <f>FALSE()</f>
@@ -31247,7 +31247,7 @@
       </c>
       <c r="D21" s="1">
         <f>VLOOKUP(B21,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E21" s="3">
         <f t="shared" si="0"/>
@@ -31255,7 +31255,7 @@
       </c>
       <c r="F21" s="1">
         <f>VLOOKUP(B21,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G21" s="1" t="b">
         <f>FALSE()</f>
@@ -31275,7 +31275,7 @@
       </c>
       <c r="D22" s="1">
         <f>VLOOKUP(B22,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E22" s="3">
         <f t="shared" si="0"/>
@@ -31283,7 +31283,7 @@
       </c>
       <c r="F22" s="1">
         <f>VLOOKUP(B22,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G22" s="1" t="b">
         <f>FALSE()</f>
@@ -31303,7 +31303,7 @@
       </c>
       <c r="D23" s="1">
         <f>VLOOKUP(B23,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E23" s="3">
         <f t="shared" si="0"/>
@@ -31311,7 +31311,7 @@
       </c>
       <c r="F23" s="1">
         <f>VLOOKUP(B23,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G23" s="1" t="b">
         <f>FALSE()</f>
@@ -31331,7 +31331,7 @@
       </c>
       <c r="D24" s="1">
         <f>VLOOKUP(B24,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E24" s="3">
         <f t="shared" si="0"/>
@@ -31339,7 +31339,7 @@
       </c>
       <c r="F24" s="1">
         <f>VLOOKUP(B24,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G24" s="1" t="b">
         <f>FALSE()</f>
@@ -31359,7 +31359,7 @@
       </c>
       <c r="D25" s="1">
         <f>VLOOKUP(B25,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E25" s="3">
         <f t="shared" si="0"/>
@@ -31367,7 +31367,7 @@
       </c>
       <c r="F25" s="1">
         <f>VLOOKUP(B25,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G25" s="1" t="b">
         <f>FALSE()</f>
@@ -31387,7 +31387,7 @@
       </c>
       <c r="D26" s="1">
         <f>VLOOKUP(B26,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E26" s="3">
         <f t="shared" si="0"/>
@@ -31395,7 +31395,7 @@
       </c>
       <c r="F26" s="1">
         <f>VLOOKUP(B26,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G26" s="1" t="b">
         <f>FALSE()</f>
@@ -31415,7 +31415,7 @@
       </c>
       <c r="D27" s="1">
         <f>VLOOKUP(B27,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E27" s="3">
         <f t="shared" si="0"/>
@@ -31423,7 +31423,7 @@
       </c>
       <c r="F27" s="1">
         <f>VLOOKUP(B27,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G27" s="1" t="b">
         <f>FALSE()</f>
@@ -31443,7 +31443,7 @@
       </c>
       <c r="D28" s="1">
         <f>VLOOKUP(B28,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E28" s="3">
         <f t="shared" si="0"/>
@@ -31451,7 +31451,7 @@
       </c>
       <c r="F28" s="1">
         <f>VLOOKUP(B28,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G28" s="1" t="b">
         <f>FALSE()</f>
@@ -50343,7 +50343,7 @@
       </c>
       <c r="D703" s="1">
         <f>VLOOKUP(B703,StdInfo!B:E,2,FALSE())</f>
-        <v>4.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="E703" s="3">
         <f t="shared" si="20"/>
@@ -50351,7 +50351,7 @@
       </c>
       <c r="F703" s="1">
         <f>VLOOKUP(B703,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G703" s="1" t="b">
         <f t="shared" si="21"/>
@@ -50371,7 +50371,7 @@
       </c>
       <c r="D704" s="1">
         <f>VLOOKUP(B704,StdInfo!B:E,2,FALSE())</f>
-        <v>4.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="E704" s="3">
         <f t="shared" si="20"/>
@@ -50379,7 +50379,7 @@
       </c>
       <c r="F704" s="1">
         <f>VLOOKUP(B704,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G704" s="1" t="b">
         <f t="shared" si="21"/>
@@ -50399,7 +50399,7 @@
       </c>
       <c r="D705" s="1">
         <f>VLOOKUP(B705,StdInfo!B:E,2,FALSE())</f>
-        <v>4.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="E705" s="3">
         <f t="shared" si="20"/>
@@ -50407,7 +50407,7 @@
       </c>
       <c r="F705" s="1">
         <f>VLOOKUP(B705,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G705" s="1" t="b">
         <f t="shared" si="21"/>
@@ -50427,7 +50427,7 @@
       </c>
       <c r="D706" s="1">
         <f>VLOOKUP(B706,StdInfo!B:E,2,FALSE())</f>
-        <v>4.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="E706" s="3">
         <f t="shared" ref="E706:E769" si="22">ROUND(D706/C706*100000*F706/2.5,10)/IF(G706=TRUE(),2,1)</f>
@@ -50435,7 +50435,7 @@
       </c>
       <c r="F706" s="1">
         <f>VLOOKUP(B706,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G706" s="1" t="b">
         <f t="shared" si="21"/>
@@ -50455,7 +50455,7 @@
       </c>
       <c r="D707" s="1">
         <f>VLOOKUP(B707,StdInfo!B:E,2,FALSE())</f>
-        <v>4.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="E707" s="3">
         <f t="shared" si="22"/>
@@ -50463,7 +50463,7 @@
       </c>
       <c r="F707" s="1">
         <f>VLOOKUP(B707,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G707" s="1" t="b">
         <f t="shared" si="21"/>
@@ -50483,7 +50483,7 @@
       </c>
       <c r="D708" s="1">
         <f>VLOOKUP(B708,StdInfo!B:E,2,FALSE())</f>
-        <v>4.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="E708" s="3">
         <f t="shared" si="22"/>
@@ -50491,7 +50491,7 @@
       </c>
       <c r="F708" s="1">
         <f>VLOOKUP(B708,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G708" s="1" t="b">
         <f t="shared" si="21"/>
@@ -50511,7 +50511,7 @@
       </c>
       <c r="D709" s="1">
         <f>VLOOKUP(B709,StdInfo!B:E,2,FALSE())</f>
-        <v>4.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="E709" s="3">
         <f t="shared" si="22"/>
@@ -50519,7 +50519,7 @@
       </c>
       <c r="F709" s="1">
         <f>VLOOKUP(B709,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G709" s="1" t="b">
         <f t="shared" si="21"/>
@@ -50539,7 +50539,7 @@
       </c>
       <c r="D710" s="1">
         <f>VLOOKUP(B710,StdInfo!B:E,2,FALSE())</f>
-        <v>4.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="E710" s="3">
         <f t="shared" si="22"/>
@@ -50547,7 +50547,7 @@
       </c>
       <c r="F710" s="1">
         <f>VLOOKUP(B710,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G710" s="1" t="b">
         <f t="shared" si="21"/>
@@ -50567,7 +50567,7 @@
       </c>
       <c r="D711" s="1">
         <f>VLOOKUP(B711,StdInfo!B:E,2,FALSE())</f>
-        <v>4.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="E711" s="3">
         <f t="shared" si="22"/>
@@ -50575,7 +50575,7 @@
       </c>
       <c r="F711" s="1">
         <f>VLOOKUP(B711,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G711" s="1" t="b">
         <f t="shared" si="21"/>
@@ -50595,7 +50595,7 @@
       </c>
       <c r="D712" s="1">
         <f>VLOOKUP(B712,StdInfo!B:E,2,FALSE())</f>
-        <v>4.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="E712" s="3">
         <f t="shared" si="22"/>
@@ -50603,7 +50603,7 @@
       </c>
       <c r="F712" s="1">
         <f>VLOOKUP(B712,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G712" s="1" t="b">
         <f t="shared" si="21"/>
@@ -50623,7 +50623,7 @@
       </c>
       <c r="D713" s="1">
         <f>VLOOKUP(B713,StdInfo!B:E,2,FALSE())</f>
-        <v>4.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="E713" s="3">
         <f t="shared" si="22"/>
@@ -50631,7 +50631,7 @@
       </c>
       <c r="F713" s="1">
         <f>VLOOKUP(B713,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G713" s="1" t="b">
         <f t="shared" si="21"/>
@@ -50651,7 +50651,7 @@
       </c>
       <c r="D714" s="1">
         <f>VLOOKUP(B714,StdInfo!B:E,2,FALSE())</f>
-        <v>4.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="E714" s="3">
         <f t="shared" si="22"/>
@@ -50659,7 +50659,7 @@
       </c>
       <c r="F714" s="1">
         <f>VLOOKUP(B714,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G714" s="1" t="b">
         <f t="shared" si="21"/>
@@ -50679,7 +50679,7 @@
       </c>
       <c r="D715" s="1">
         <f>VLOOKUP(B715,StdInfo!B:E,2,FALSE())</f>
-        <v>4.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="E715" s="3">
         <f t="shared" si="22"/>
@@ -50687,7 +50687,7 @@
       </c>
       <c r="F715" s="1">
         <f>VLOOKUP(B715,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G715" s="1" t="b">
         <f t="shared" si="21"/>
@@ -50707,7 +50707,7 @@
       </c>
       <c r="D716" s="1">
         <f>VLOOKUP(B716,StdInfo!B:E,2,FALSE())</f>
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
       <c r="E716" s="3">
         <f t="shared" si="22"/>
@@ -50715,7 +50715,7 @@
       </c>
       <c r="F716" s="1">
         <f>VLOOKUP(B716,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G716" s="1" t="b">
         <f t="shared" si="21"/>
@@ -50735,7 +50735,7 @@
       </c>
       <c r="D717" s="1">
         <f>VLOOKUP(B717,StdInfo!B:E,2,FALSE())</f>
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
       <c r="E717" s="3">
         <f t="shared" si="22"/>
@@ -50743,7 +50743,7 @@
       </c>
       <c r="F717" s="1">
         <f>VLOOKUP(B717,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G717" s="1" t="b">
         <f t="shared" si="21"/>
@@ -50763,7 +50763,7 @@
       </c>
       <c r="D718" s="1">
         <f>VLOOKUP(B718,StdInfo!B:E,2,FALSE())</f>
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
       <c r="E718" s="3">
         <f t="shared" si="22"/>
@@ -50771,7 +50771,7 @@
       </c>
       <c r="F718" s="1">
         <f>VLOOKUP(B718,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G718" s="1" t="b">
         <f t="shared" si="21"/>
@@ -50791,7 +50791,7 @@
       </c>
       <c r="D719" s="1">
         <f>VLOOKUP(B719,StdInfo!B:E,2,FALSE())</f>
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
       <c r="E719" s="3">
         <f t="shared" si="22"/>
@@ -50799,7 +50799,7 @@
       </c>
       <c r="F719" s="1">
         <f>VLOOKUP(B719,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G719" s="1" t="b">
         <f t="shared" si="21"/>
@@ -50819,7 +50819,7 @@
       </c>
       <c r="D720" s="1">
         <f>VLOOKUP(B720,StdInfo!B:E,2,FALSE())</f>
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
       <c r="E720" s="3">
         <f t="shared" si="22"/>
@@ -50827,7 +50827,7 @@
       </c>
       <c r="F720" s="1">
         <f>VLOOKUP(B720,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G720" s="1" t="b">
         <f t="shared" si="21"/>
@@ -50847,7 +50847,7 @@
       </c>
       <c r="D721" s="1">
         <f>VLOOKUP(B721,StdInfo!B:E,2,FALSE())</f>
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
       <c r="E721" s="3">
         <f t="shared" si="22"/>
@@ -50855,7 +50855,7 @@
       </c>
       <c r="F721" s="1">
         <f>VLOOKUP(B721,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G721" s="1" t="b">
         <f t="shared" si="21"/>
@@ -50875,7 +50875,7 @@
       </c>
       <c r="D722" s="1">
         <f>VLOOKUP(B722,StdInfo!B:E,2,FALSE())</f>
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
       <c r="E722" s="3">
         <f t="shared" si="22"/>
@@ -50883,7 +50883,7 @@
       </c>
       <c r="F722" s="1">
         <f>VLOOKUP(B722,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G722" s="1" t="b">
         <f t="shared" si="21"/>
@@ -50903,7 +50903,7 @@
       </c>
       <c r="D723" s="1">
         <f>VLOOKUP(B723,StdInfo!B:E,2,FALSE())</f>
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
       <c r="E723" s="3">
         <f t="shared" si="22"/>
@@ -50911,7 +50911,7 @@
       </c>
       <c r="F723" s="1">
         <f>VLOOKUP(B723,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G723" s="1" t="b">
         <f t="shared" si="21"/>
@@ -50931,7 +50931,7 @@
       </c>
       <c r="D724" s="1">
         <f>VLOOKUP(B724,StdInfo!B:E,2,FALSE())</f>
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
       <c r="E724" s="3">
         <f t="shared" si="22"/>
@@ -50939,7 +50939,7 @@
       </c>
       <c r="F724" s="1">
         <f>VLOOKUP(B724,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G724" s="1" t="b">
         <f t="shared" si="21"/>
@@ -50959,7 +50959,7 @@
       </c>
       <c r="D725" s="1">
         <f>VLOOKUP(B725,StdInfo!B:E,2,FALSE())</f>
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
       <c r="E725" s="3">
         <f t="shared" si="22"/>
@@ -50967,7 +50967,7 @@
       </c>
       <c r="F725" s="1">
         <f>VLOOKUP(B725,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G725" s="1" t="b">
         <f t="shared" si="21"/>
@@ -50987,7 +50987,7 @@
       </c>
       <c r="D726" s="1">
         <f>VLOOKUP(B726,StdInfo!B:E,2,FALSE())</f>
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
       <c r="E726" s="3">
         <f t="shared" si="22"/>
@@ -50995,7 +50995,7 @@
       </c>
       <c r="F726" s="1">
         <f>VLOOKUP(B726,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G726" s="1" t="b">
         <f t="shared" si="21"/>
@@ -51015,7 +51015,7 @@
       </c>
       <c r="D727" s="1">
         <f>VLOOKUP(B727,StdInfo!B:E,2,FALSE())</f>
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
       <c r="E727" s="3">
         <f t="shared" si="22"/>
@@ -51023,7 +51023,7 @@
       </c>
       <c r="F727" s="1">
         <f>VLOOKUP(B727,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G727" s="1" t="b">
         <f t="shared" si="21"/>
@@ -51043,7 +51043,7 @@
       </c>
       <c r="D728" s="1">
         <f>VLOOKUP(B728,StdInfo!B:E,2,FALSE())</f>
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
       <c r="E728" s="3">
         <f t="shared" si="22"/>
@@ -51051,7 +51051,7 @@
       </c>
       <c r="F728" s="1">
         <f>VLOOKUP(B728,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G728" s="1" t="b">
         <f t="shared" si="21"/>
@@ -51071,7 +51071,7 @@
       </c>
       <c r="D729" s="1">
         <f>VLOOKUP(B729,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E729" s="3">
         <f t="shared" si="22"/>
@@ -51079,7 +51079,7 @@
       </c>
       <c r="F729" s="1">
         <f>VLOOKUP(B729,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G729" s="1" t="b">
         <f t="shared" si="21"/>
@@ -51099,7 +51099,7 @@
       </c>
       <c r="D730" s="1">
         <f>VLOOKUP(B730,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E730" s="3">
         <f t="shared" si="22"/>
@@ -51107,7 +51107,7 @@
       </c>
       <c r="F730" s="1">
         <f>VLOOKUP(B730,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G730" s="1" t="b">
         <f t="shared" si="21"/>
@@ -51127,7 +51127,7 @@
       </c>
       <c r="D731" s="1">
         <f>VLOOKUP(B731,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E731" s="3">
         <f t="shared" si="22"/>
@@ -51135,7 +51135,7 @@
       </c>
       <c r="F731" s="1">
         <f>VLOOKUP(B731,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G731" s="1" t="b">
         <f t="shared" si="21"/>
@@ -51155,7 +51155,7 @@
       </c>
       <c r="D732" s="1">
         <f>VLOOKUP(B732,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E732" s="3">
         <f t="shared" si="22"/>
@@ -51163,7 +51163,7 @@
       </c>
       <c r="F732" s="1">
         <f>VLOOKUP(B732,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G732" s="1" t="b">
         <f t="shared" si="21"/>
@@ -51183,7 +51183,7 @@
       </c>
       <c r="D733" s="1">
         <f>VLOOKUP(B733,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E733" s="3">
         <f t="shared" si="22"/>
@@ -51191,7 +51191,7 @@
       </c>
       <c r="F733" s="1">
         <f>VLOOKUP(B733,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G733" s="1" t="b">
         <f t="shared" si="21"/>
@@ -51211,7 +51211,7 @@
       </c>
       <c r="D734" s="1">
         <f>VLOOKUP(B734,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E734" s="3">
         <f t="shared" si="22"/>
@@ -51219,7 +51219,7 @@
       </c>
       <c r="F734" s="1">
         <f>VLOOKUP(B734,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G734" s="1" t="b">
         <f t="shared" si="21"/>
@@ -51239,7 +51239,7 @@
       </c>
       <c r="D735" s="1">
         <f>VLOOKUP(B735,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E735" s="3">
         <f t="shared" si="22"/>
@@ -51247,7 +51247,7 @@
       </c>
       <c r="F735" s="1">
         <f>VLOOKUP(B735,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G735" s="1" t="b">
         <f t="shared" si="21"/>
@@ -51267,7 +51267,7 @@
       </c>
       <c r="D736" s="1">
         <f>VLOOKUP(B736,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E736" s="3">
         <f t="shared" si="22"/>
@@ -51275,7 +51275,7 @@
       </c>
       <c r="F736" s="1">
         <f>VLOOKUP(B736,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G736" s="1" t="b">
         <f t="shared" si="21"/>
@@ -51295,7 +51295,7 @@
       </c>
       <c r="D737" s="1">
         <f>VLOOKUP(B737,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E737" s="3">
         <f t="shared" si="22"/>
@@ -51303,7 +51303,7 @@
       </c>
       <c r="F737" s="1">
         <f>VLOOKUP(B737,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G737" s="1" t="b">
         <f t="shared" si="21"/>
@@ -51323,7 +51323,7 @@
       </c>
       <c r="D738" s="1">
         <f>VLOOKUP(B738,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E738" s="3">
         <f t="shared" si="22"/>
@@ -51331,7 +51331,7 @@
       </c>
       <c r="F738" s="1">
         <f>VLOOKUP(B738,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G738" s="1" t="b">
         <f t="shared" si="21"/>
@@ -51351,7 +51351,7 @@
       </c>
       <c r="D739" s="1">
         <f>VLOOKUP(B739,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E739" s="3">
         <f t="shared" si="22"/>
@@ -51359,7 +51359,7 @@
       </c>
       <c r="F739" s="1">
         <f>VLOOKUP(B739,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G739" s="1" t="b">
         <f t="shared" si="21"/>
@@ -51379,7 +51379,7 @@
       </c>
       <c r="D740" s="1">
         <f>VLOOKUP(B740,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E740" s="3">
         <f t="shared" si="22"/>
@@ -51387,7 +51387,7 @@
       </c>
       <c r="F740" s="1">
         <f>VLOOKUP(B740,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G740" s="1" t="b">
         <f t="shared" si="21"/>
@@ -51407,7 +51407,7 @@
       </c>
       <c r="D741" s="1">
         <f>VLOOKUP(B741,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E741" s="3">
         <f t="shared" si="22"/>
@@ -51415,7 +51415,7 @@
       </c>
       <c r="F741" s="1">
         <f>VLOOKUP(B741,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G741" s="1" t="b">
         <f t="shared" si="21"/>
@@ -51435,7 +51435,7 @@
       </c>
       <c r="D742" s="1">
         <f>VLOOKUP(B742,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="E742" s="3">
         <f t="shared" si="22"/>
@@ -51443,7 +51443,7 @@
       </c>
       <c r="F742" s="1">
         <f>VLOOKUP(B742,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="G742" s="1" t="b">
         <f t="shared" si="21"/>
@@ -51463,7 +51463,7 @@
       </c>
       <c r="D743" s="1">
         <f>VLOOKUP(B743,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="E743" s="3">
         <f t="shared" si="22"/>
@@ -51471,7 +51471,7 @@
       </c>
       <c r="F743" s="1">
         <f>VLOOKUP(B743,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="G743" s="1" t="b">
         <f t="shared" si="21"/>
@@ -51491,7 +51491,7 @@
       </c>
       <c r="D744" s="1">
         <f>VLOOKUP(B744,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="E744" s="3">
         <f t="shared" si="22"/>
@@ -51499,7 +51499,7 @@
       </c>
       <c r="F744" s="1">
         <f>VLOOKUP(B744,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="G744" s="1" t="b">
         <f t="shared" si="21"/>
@@ -51519,7 +51519,7 @@
       </c>
       <c r="D745" s="1">
         <f>VLOOKUP(B745,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="E745" s="3">
         <f t="shared" si="22"/>
@@ -51527,7 +51527,7 @@
       </c>
       <c r="F745" s="1">
         <f>VLOOKUP(B745,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="G745" s="1" t="b">
         <f t="shared" si="21"/>
@@ -51547,7 +51547,7 @@
       </c>
       <c r="D746" s="1">
         <f>VLOOKUP(B746,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="E746" s="3">
         <f t="shared" si="22"/>
@@ -51555,7 +51555,7 @@
       </c>
       <c r="F746" s="1">
         <f>VLOOKUP(B746,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="G746" s="1" t="b">
         <f t="shared" si="21"/>
@@ -51575,7 +51575,7 @@
       </c>
       <c r="D747" s="1">
         <f>VLOOKUP(B747,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="E747" s="3">
         <f t="shared" si="22"/>
@@ -51583,7 +51583,7 @@
       </c>
       <c r="F747" s="1">
         <f>VLOOKUP(B747,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="G747" s="1" t="b">
         <f t="shared" si="21"/>
@@ -51603,7 +51603,7 @@
       </c>
       <c r="D748" s="1">
         <f>VLOOKUP(B748,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="E748" s="3">
         <f t="shared" si="22"/>
@@ -51611,7 +51611,7 @@
       </c>
       <c r="F748" s="1">
         <f>VLOOKUP(B748,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="G748" s="1" t="b">
         <f t="shared" si="21"/>
@@ -51631,7 +51631,7 @@
       </c>
       <c r="D749" s="1">
         <f>VLOOKUP(B749,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="E749" s="3">
         <f t="shared" si="22"/>
@@ -51639,7 +51639,7 @@
       </c>
       <c r="F749" s="1">
         <f>VLOOKUP(B749,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="G749" s="1" t="b">
         <f t="shared" si="21"/>
@@ -51659,7 +51659,7 @@
       </c>
       <c r="D750" s="1">
         <f>VLOOKUP(B750,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="E750" s="3">
         <f t="shared" si="22"/>
@@ -51667,7 +51667,7 @@
       </c>
       <c r="F750" s="1">
         <f>VLOOKUP(B750,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="G750" s="1" t="b">
         <f t="shared" si="21"/>
@@ -51687,7 +51687,7 @@
       </c>
       <c r="D751" s="1">
         <f>VLOOKUP(B751,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="E751" s="3">
         <f t="shared" si="22"/>
@@ -51695,7 +51695,7 @@
       </c>
       <c r="F751" s="1">
         <f>VLOOKUP(B751,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="G751" s="1" t="b">
         <f t="shared" si="21"/>
@@ -51715,7 +51715,7 @@
       </c>
       <c r="D752" s="1">
         <f>VLOOKUP(B752,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="E752" s="3">
         <f t="shared" si="22"/>
@@ -51723,7 +51723,7 @@
       </c>
       <c r="F752" s="1">
         <f>VLOOKUP(B752,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="G752" s="1" t="b">
         <f t="shared" si="21"/>
@@ -51743,7 +51743,7 @@
       </c>
       <c r="D753" s="1">
         <f>VLOOKUP(B753,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="E753" s="3">
         <f t="shared" si="22"/>
@@ -51751,7 +51751,7 @@
       </c>
       <c r="F753" s="1">
         <f>VLOOKUP(B753,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="G753" s="1" t="b">
         <f t="shared" si="21"/>
@@ -51771,7 +51771,7 @@
       </c>
       <c r="D754" s="1">
         <f>VLOOKUP(B754,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="E754" s="3">
         <f t="shared" si="22"/>
@@ -51779,7 +51779,7 @@
       </c>
       <c r="F754" s="1">
         <f>VLOOKUP(B754,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="G754" s="1" t="b">
         <f t="shared" si="21"/>
@@ -51799,7 +51799,7 @@
       </c>
       <c r="D755" s="1">
         <f>VLOOKUP(B755,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="E755" s="3">
         <f t="shared" si="22"/>
@@ -51807,7 +51807,7 @@
       </c>
       <c r="F755" s="1">
         <f>VLOOKUP(B755,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="G755" s="1" t="b">
         <f t="shared" si="21"/>
@@ -51827,7 +51827,7 @@
       </c>
       <c r="D756" s="1">
         <f>VLOOKUP(B756,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="E756" s="3">
         <f t="shared" si="22"/>
@@ -51835,7 +51835,7 @@
       </c>
       <c r="F756" s="1">
         <f>VLOOKUP(B756,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="G756" s="1" t="b">
         <f t="shared" si="21"/>
@@ -51855,7 +51855,7 @@
       </c>
       <c r="D757" s="1">
         <f>VLOOKUP(B757,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="E757" s="3">
         <f t="shared" si="22"/>
@@ -51863,7 +51863,7 @@
       </c>
       <c r="F757" s="1">
         <f>VLOOKUP(B757,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="G757" s="1" t="b">
         <f t="shared" si="21"/>
@@ -51883,7 +51883,7 @@
       </c>
       <c r="D758" s="1">
         <f>VLOOKUP(B758,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="E758" s="3">
         <f t="shared" si="22"/>
@@ -51891,7 +51891,7 @@
       </c>
       <c r="F758" s="1">
         <f>VLOOKUP(B758,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="G758" s="1" t="b">
         <f t="shared" ref="G758:G821" si="23">MID(A758,4,4)=MID(A758,9,4)</f>
@@ -51911,7 +51911,7 @@
       </c>
       <c r="D759" s="1">
         <f>VLOOKUP(B759,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="E759" s="3">
         <f t="shared" si="22"/>
@@ -51919,7 +51919,7 @@
       </c>
       <c r="F759" s="1">
         <f>VLOOKUP(B759,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="G759" s="1" t="b">
         <f t="shared" si="23"/>
@@ -51939,7 +51939,7 @@
       </c>
       <c r="D760" s="1">
         <f>VLOOKUP(B760,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="E760" s="3">
         <f t="shared" si="22"/>
@@ -51947,7 +51947,7 @@
       </c>
       <c r="F760" s="1">
         <f>VLOOKUP(B760,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="G760" s="1" t="b">
         <f t="shared" si="23"/>
@@ -51967,7 +51967,7 @@
       </c>
       <c r="D761" s="1">
         <f>VLOOKUP(B761,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="E761" s="3">
         <f t="shared" si="22"/>
@@ -51975,7 +51975,7 @@
       </c>
       <c r="F761" s="1">
         <f>VLOOKUP(B761,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="G761" s="1" t="b">
         <f t="shared" si="23"/>
@@ -51995,7 +51995,7 @@
       </c>
       <c r="D762" s="1">
         <f>VLOOKUP(B762,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="E762" s="3">
         <f t="shared" si="22"/>
@@ -52003,7 +52003,7 @@
       </c>
       <c r="F762" s="1">
         <f>VLOOKUP(B762,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="G762" s="1" t="b">
         <f t="shared" si="23"/>
@@ -52023,7 +52023,7 @@
       </c>
       <c r="D763" s="1">
         <f>VLOOKUP(B763,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="E763" s="3">
         <f t="shared" si="22"/>
@@ -52031,7 +52031,7 @@
       </c>
       <c r="F763" s="1">
         <f>VLOOKUP(B763,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="G763" s="1" t="b">
         <f t="shared" si="23"/>
@@ -52051,7 +52051,7 @@
       </c>
       <c r="D764" s="1">
         <f>VLOOKUP(B764,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="E764" s="3">
         <f t="shared" si="22"/>
@@ -52059,7 +52059,7 @@
       </c>
       <c r="F764" s="1">
         <f>VLOOKUP(B764,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="G764" s="1" t="b">
         <f t="shared" si="23"/>
@@ -52079,7 +52079,7 @@
       </c>
       <c r="D765" s="1">
         <f>VLOOKUP(B765,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="E765" s="3">
         <f t="shared" si="22"/>
@@ -52087,7 +52087,7 @@
       </c>
       <c r="F765" s="1">
         <f>VLOOKUP(B765,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="G765" s="1" t="b">
         <f t="shared" si="23"/>
@@ -52107,7 +52107,7 @@
       </c>
       <c r="D766" s="1">
         <f>VLOOKUP(B766,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="E766" s="3">
         <f t="shared" si="22"/>
@@ -52115,7 +52115,7 @@
       </c>
       <c r="F766" s="1">
         <f>VLOOKUP(B766,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="G766" s="1" t="b">
         <f t="shared" si="23"/>
@@ -52135,7 +52135,7 @@
       </c>
       <c r="D767" s="1">
         <f>VLOOKUP(B767,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="E767" s="3">
         <f t="shared" si="22"/>
@@ -52143,7 +52143,7 @@
       </c>
       <c r="F767" s="1">
         <f>VLOOKUP(B767,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="G767" s="1" t="b">
         <f t="shared" si="23"/>
@@ -52163,7 +52163,7 @@
       </c>
       <c r="D768" s="1">
         <f>VLOOKUP(B768,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="E768" s="3">
         <f t="shared" si="22"/>
@@ -52171,7 +52171,7 @@
       </c>
       <c r="F768" s="1">
         <f>VLOOKUP(B768,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="G768" s="1" t="b">
         <f t="shared" si="23"/>
@@ -52191,7 +52191,7 @@
       </c>
       <c r="D769" s="1">
         <f>VLOOKUP(B769,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="E769" s="3">
         <f t="shared" si="22"/>
@@ -52199,7 +52199,7 @@
       </c>
       <c r="F769" s="1">
         <f>VLOOKUP(B769,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="G769" s="1" t="b">
         <f t="shared" si="23"/>
@@ -52219,7 +52219,7 @@
       </c>
       <c r="D770" s="1">
         <f>VLOOKUP(B770,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="E770" s="3">
         <f t="shared" ref="E770:E833" si="24">ROUND(D770/C770*100000*F770/2.5,10)/IF(G770=TRUE(),2,1)</f>
@@ -52227,7 +52227,7 @@
       </c>
       <c r="F770" s="1">
         <f>VLOOKUP(B770,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="G770" s="1" t="b">
         <f t="shared" si="23"/>
@@ -52247,7 +52247,7 @@
       </c>
       <c r="D771" s="1">
         <f>VLOOKUP(B771,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="E771" s="3">
         <f t="shared" si="24"/>
@@ -52255,7 +52255,7 @@
       </c>
       <c r="F771" s="1">
         <f>VLOOKUP(B771,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="G771" s="1" t="b">
         <f t="shared" si="23"/>
@@ -52275,7 +52275,7 @@
       </c>
       <c r="D772" s="1">
         <f>VLOOKUP(B772,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="E772" s="3">
         <f t="shared" si="24"/>
@@ -52283,7 +52283,7 @@
       </c>
       <c r="F772" s="1">
         <f>VLOOKUP(B772,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="G772" s="1" t="b">
         <f t="shared" si="23"/>
@@ -52303,7 +52303,7 @@
       </c>
       <c r="D773" s="1">
         <f>VLOOKUP(B773,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="E773" s="3">
         <f t="shared" si="24"/>
@@ -52311,7 +52311,7 @@
       </c>
       <c r="F773" s="1">
         <f>VLOOKUP(B773,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="G773" s="1" t="b">
         <f t="shared" si="23"/>
@@ -52331,7 +52331,7 @@
       </c>
       <c r="D774" s="1">
         <f>VLOOKUP(B774,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="E774" s="3">
         <f t="shared" si="24"/>
@@ -52339,7 +52339,7 @@
       </c>
       <c r="F774" s="1">
         <f>VLOOKUP(B774,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="G774" s="1" t="b">
         <f t="shared" si="23"/>
@@ -52359,7 +52359,7 @@
       </c>
       <c r="D775" s="1">
         <f>VLOOKUP(B775,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="E775" s="3">
         <f t="shared" si="24"/>
@@ -52367,7 +52367,7 @@
       </c>
       <c r="F775" s="1">
         <f>VLOOKUP(B775,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="G775" s="1" t="b">
         <f t="shared" si="23"/>
@@ -52387,7 +52387,7 @@
       </c>
       <c r="D776" s="1">
         <f>VLOOKUP(B776,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="E776" s="3">
         <f t="shared" si="24"/>
@@ -52395,7 +52395,7 @@
       </c>
       <c r="F776" s="1">
         <f>VLOOKUP(B776,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="G776" s="1" t="b">
         <f t="shared" si="23"/>
@@ -52415,7 +52415,7 @@
       </c>
       <c r="D777" s="1">
         <f>VLOOKUP(B777,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="E777" s="3">
         <f t="shared" si="24"/>
@@ -52423,7 +52423,7 @@
       </c>
       <c r="F777" s="1">
         <f>VLOOKUP(B777,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="G777" s="1" t="b">
         <f t="shared" si="23"/>
@@ -52443,7 +52443,7 @@
       </c>
       <c r="D778" s="1">
         <f>VLOOKUP(B778,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="E778" s="3">
         <f t="shared" si="24"/>
@@ -52451,7 +52451,7 @@
       </c>
       <c r="F778" s="1">
         <f>VLOOKUP(B778,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="G778" s="1" t="b">
         <f t="shared" si="23"/>
@@ -52471,7 +52471,7 @@
       </c>
       <c r="D779" s="1">
         <f>VLOOKUP(B779,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="E779" s="3">
         <f t="shared" si="24"/>
@@ -52479,7 +52479,7 @@
       </c>
       <c r="F779" s="1">
         <f>VLOOKUP(B779,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="G779" s="1" t="b">
         <f t="shared" si="23"/>
@@ -52499,7 +52499,7 @@
       </c>
       <c r="D780" s="1">
         <f>VLOOKUP(B780,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="E780" s="3">
         <f t="shared" si="24"/>
@@ -52507,7 +52507,7 @@
       </c>
       <c r="F780" s="1">
         <f>VLOOKUP(B780,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="G780" s="1" t="b">
         <f t="shared" si="23"/>
@@ -52527,7 +52527,7 @@
       </c>
       <c r="D781" s="1">
         <f>VLOOKUP(B781,StdInfo!B:E,2,FALSE())</f>
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="E781" s="3">
         <f t="shared" si="24"/>
@@ -52535,7 +52535,7 @@
       </c>
       <c r="F781" s="1">
         <f>VLOOKUP(B781,StdInfo!B:E,3,FALSE())</f>
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="G781" s="1" t="b">
         <f t="shared" si="23"/>
@@ -56583,8 +56583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F173"/>
   <sheetViews>
-    <sheetView topLeftCell="A130" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E151" sqref="E151"/>
+    <sheetView tabSelected="1" topLeftCell="A130" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F146" sqref="F146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -58364,23 +58364,27 @@
       </c>
       <c r="C134" s="1"/>
     </row>
-    <row r="135" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>1800</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>1015</v>
       </c>
-      <c r="C135" s="58">
-        <v>0.04</v>
+      <c r="C135" s="1">
+        <v>1</v>
       </c>
       <c r="D135" s="1">
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="E135" s="1">
         <v>689.49900000000002</v>
       </c>
       <c r="F135" s="1"/>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C136" s="11"/>
+      <c r="D136" s="11"/>
     </row>
     <row r="137" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A137" s="61" t="s">
@@ -58390,14 +58394,18 @@
         <v>976</v>
       </c>
       <c r="C137" s="58">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="D137" s="1">
-        <v>2.5</v>
+        <v>0.01</v>
+      </c>
+      <c r="D137" s="11">
+        <v>1</v>
       </c>
       <c r="E137" s="62">
         <v>504.52</v>
       </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C138" s="11"/>
+      <c r="D138" s="11"/>
     </row>
     <row r="139" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A139" s="63" t="s">
@@ -58407,31 +58415,39 @@
         <v>989</v>
       </c>
       <c r="C139" s="58">
-        <v>0.08</v>
-      </c>
-      <c r="D139" s="1">
-        <v>2.5</v>
+        <v>0.2</v>
+      </c>
+      <c r="D139" s="11">
+        <v>1</v>
       </c>
       <c r="E139" s="3">
         <v>692.59</v>
       </c>
     </row>
-    <row r="141" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C140" s="11"/>
+      <c r="D140" s="11"/>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="64" t="s">
         <v>1803</v>
       </c>
       <c r="B141" s="42" t="s">
         <v>1002</v>
       </c>
-      <c r="C141" s="58">
-        <v>0.04</v>
-      </c>
-      <c r="D141" s="1">
-        <v>2.5</v>
+      <c r="C141" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="D141" s="11">
+        <v>1</v>
       </c>
       <c r="E141" s="65">
         <v>854.65</v>
       </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C142" s="11"/>
+      <c r="D142" s="11"/>
     </row>
     <row r="143" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A143" s="66" t="s">
@@ -58441,10 +58457,10 @@
         <v>835</v>
       </c>
       <c r="C143" s="52">
-        <v>0.04</v>
-      </c>
-      <c r="D143" s="1">
-        <v>2.5</v>
+        <v>0.1</v>
+      </c>
+      <c r="D143" s="11">
+        <v>1</v>
       </c>
       <c r="E143">
         <v>291.31200000000001</v>
@@ -58460,7 +58476,7 @@
       <c r="C144" s="52">
         <v>0.2</v>
       </c>
-      <c r="D144">
+      <c r="D144" s="11">
         <v>1</v>
       </c>
       <c r="E144">

</xml_diff>